<commit_message>
some update on pitchdeck
</commit_message>
<xml_diff>
--- a/business/business-plan/src/market-size.xlsx
+++ b/business/business-plan/src/market-size.xlsx
@@ -1,36 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\xampp\htdocs\projects\talambar_cdn\business\investment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\web\projects\talambar_cdn\business\business-plan\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9505803-5270-4EAD-AA5C-1B47160198F4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAD33BAA-76EC-45C1-9C85-846127A2FAA0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3375" yWindow="2025" windowWidth="28800" windowHeight="11385" xr2:uid="{C0925052-1D72-4D4B-B1F6-A52D18756B59}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C0925052-1D72-4D4B-B1F6-A52D18756B59}"/>
   </bookViews>
   <sheets>
     <sheet name="Market Size" sheetId="1" r:id="rId1"/>
+    <sheet name="Market Size till 2031" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="13">
   <si>
     <t>Year</t>
   </si>
@@ -114,7 +110,10 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.0"/>
     </dxf>
@@ -291,9 +290,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Market Size'!$A$2:$A$13</c:f>
+              <c:f>'Market Size'!$A$2:$A$12</c:f>
               <c:strCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>2020</c:v>
                 </c:pt>
@@ -326,19 +325,16 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>2030*</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2031*</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Market Size'!$B$2:$B$13</c:f>
+              <c:f>'Market Size'!$B$2:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>7.4</c:v>
                 </c:pt>
@@ -371,9 +367,6 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>27.928000000000001</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>31.894000000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -381,6 +374,434 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-EDB3-4031-9439-E5B433D13FD7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="80"/>
+        <c:overlap val="25"/>
+        <c:axId val="1049503743"/>
+        <c:axId val="1018175119"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1049503743"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="15875" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1018175119"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1018175119"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="20" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1049503743"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="2"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="50" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mj-lt"/>
+                <a:ea typeface="+mj-ea"/>
+                <a:cs typeface="+mj-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>e-Commerce software market revenues worldwide from 2020 to 2027</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="50" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mj-ea"/>
+              <a:cs typeface="+mj-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Market Size till 2031'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Market in million US dollars</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:alpha val="70000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Market Size till 2031'!$A$2:$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2021*</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2022*</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2023*</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2024*</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2025*</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2026*</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2027*</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2028*</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2029*</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2030*</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2031*</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Market Size till 2031'!$B$2:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>7.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.4509999999999987</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.6519999999999992</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.023</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12.588999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14.376999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16.419</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>18.751000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>21.414000000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>24.455000000000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>27.928000000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>31.894000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E6D7-48E1-A029-A8246742B9BD}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -599,7 +1020,539 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="215">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="15875" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="none" spc="20" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="bg1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="70000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="70000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="70000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="70000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" baseline="0"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="0" i="0" kern="1200" cap="none" spc="50" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="15875" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" spc="20" baseline="0"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="215">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1132,12 +2085,68 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>661987</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>71436</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60E6CD47-540B-44EF-81E5-1847036C8700}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8BA83DAC-599E-4A7D-957A-4B79799941C6}" name="Table1" displayName="Table1" ref="A1:B13" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8BA83DAC-599E-4A7D-957A-4B79799941C6}" name="Table1" displayName="Table1" ref="A1:B12" totalsRowShown="0">
+  <autoFilter ref="A1:B12" xr:uid="{59ECE4EA-269E-4E7B-A60A-59ECE0840802}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{E45A0BDF-CF11-4ED1-BE9E-44317F001A4A}" name="Year"/>
+    <tableColumn id="2" xr3:uid="{F55B7823-DD66-4EA7-896B-223D79833999}" name="Market in million US dollars" dataDxfId="1">
+      <calculatedColumnFormula>ROUNDUP(B1*1.142, 3)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FA9D33DD-CA1C-46F2-9B3A-E105CAA035F1}" name="Table13" displayName="Table13" ref="A1:B13" totalsRowShown="0">
   <autoFilter ref="A1:B13" xr:uid="{59ECE4EA-269E-4E7B-A60A-59ECE0840802}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{E45A0BDF-CF11-4ED1-BE9E-44317F001A4A}" name="Year"/>
-    <tableColumn id="2" xr3:uid="{F55B7823-DD66-4EA7-896B-223D79833999}" name="Market in million US dollars" dataDxfId="0">
+    <tableColumn id="1" xr3:uid="{2DE4963C-C748-48DD-8981-5510EABC317B}" name="Year"/>
+    <tableColumn id="2" xr3:uid="{1BDAB8F8-F50C-44AC-8D49-98CD84BA335A}" name="Market in million US dollars" dataDxfId="0">
       <calculatedColumnFormula>ROUNDUP(B1*1.142, 3)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1442,10 +2451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF8147BF-3A16-440E-8872-B34EDE10F8D0}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1555,7 +2564,135 @@
         <v>11</v>
       </c>
       <c r="B12" s="1">
-        <f t="shared" si="1"/>
+        <f>ROUNDUP(B11*1.142, 3)</f>
+        <v>27.928000000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18C73478-9429-499B-8587-9FE935AF0537}">
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="27.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2020</v>
+      </c>
+      <c r="B2" s="1">
+        <v>7.4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <f>ROUNDUP(B2*1.142, 3)</f>
+        <v>8.4509999999999987</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <f t="shared" ref="B4:B12" si="0">ROUNDUP(B3*1.142, 3)</f>
+        <v>9.6519999999999992</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
+        <f t="shared" si="0"/>
+        <v>11.023</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1">
+        <f t="shared" si="0"/>
+        <v>12.588999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1">
+        <f t="shared" si="0"/>
+        <v>14.376999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1">
+        <f t="shared" si="0"/>
+        <v>16.419</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1">
+        <f t="shared" si="0"/>
+        <v>18.751000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
+        <f t="shared" si="0"/>
+        <v>21.414000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <f t="shared" si="0"/>
+        <v>24.455000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1">
+        <f t="shared" si="0"/>
         <v>27.928000000000001</v>
       </c>
     </row>

</xml_diff>